<commit_message>
Changed C1. Updated Gerbers, sckematic and BoM
</commit_message>
<xml_diff>
--- a/Documents/Bill of Materials-GTL3_Inverter.xlsx
+++ b/Documents/Bill of Materials-GTL3_Inverter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Pathfinder\Pathfinder PCB\GTL3-Lamp-Driver\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\GTL3-Lamp-Driver.git\PCB\Project Outputs for GTL3_Inverter\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89F4A82-7A20-4487-8642-1A152F33905F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9ED81EA2-5D95-47F0-90E8-DFCA22700730}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30765" yWindow="1020" windowWidth="25125" windowHeight="13830" xr2:uid="{06734A2C-B5A8-4AB1-BC0F-86EBA69CC8FE}"/>
+    <workbookView xWindow="3015" yWindow="2835" windowWidth="24285" windowHeight="11400" xr2:uid="{935E02DD-98D4-4F44-BBEB-E94F39845EF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-GTL3_Inverter" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="65">
+  <si>
+    <t>Line #</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
   <si>
     <t>Description</t>
   </si>
@@ -44,6 +50,9 @@
     <t>Designator</t>
   </si>
   <si>
+    <t>Revision ID</t>
+  </si>
+  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -62,19 +71,28 @@
     <t>Supplier Part Number 1</t>
   </si>
   <si>
+    <t>Supplier Unit Price 1</t>
+  </si>
+  <si>
     <t>Supplier Subtotal 1</t>
   </si>
   <si>
-    <t>2220 (5750 Metric) Chip Capacitor</t>
+    <t>0.33uF 63Vac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Film Capacitors 100Vdc 0.33uF 10% AEC-Q200 </t>
   </si>
   <si>
     <t>C1</t>
   </si>
   <si>
+    <t>CMP-001-00084-1</t>
+  </si>
+  <si>
     <t>KEMET</t>
   </si>
   <si>
-    <t>LDEDD3330JA5N00</t>
+    <t>LDEED3330KA5N00</t>
   </si>
   <si>
     <t>Volume Production</t>
@@ -83,7 +101,13 @@
     <t>Digi-Key</t>
   </si>
   <si>
-    <t>399-6420-1-ND</t>
+    <t>399-12874-1-ND</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0.22µF</t>
   </si>
   <si>
     <t>CAP FILM 0.22UF 2% 50VDC 2416</t>
@@ -101,6 +125,9 @@
     <t>PCF1556CT-ND</t>
   </si>
   <si>
+    <t>100µF</t>
+  </si>
+  <si>
     <t>CAP ALUM SMD 105C 100UF 50VDC</t>
   </si>
   <si>
@@ -125,6 +152,9 @@
     <t>J1, J2</t>
   </si>
   <si>
+    <t>CMP-2000-05299-1</t>
+  </si>
+  <si>
     <t>Phoenix Contact</t>
   </si>
   <si>
@@ -140,12 +170,18 @@
     <t>L1</t>
   </si>
   <si>
+    <t>CMP-0227-00173-1</t>
+  </si>
+  <si>
     <t>Wurth Electronics</t>
   </si>
   <si>
     <t>732-1696-1-ND</t>
   </si>
   <si>
+    <t>Header 2X2</t>
+  </si>
+  <si>
     <t>Header, 2-Pin, Dual row</t>
   </si>
   <si>
@@ -161,22 +197,34 @@
     <t>Q1, Q2</t>
   </si>
   <si>
+    <t>CMP-2000-06300-1</t>
+  </si>
+  <si>
     <t>Diodes Zetex</t>
   </si>
   <si>
     <t>FZT853CT-ND</t>
   </si>
   <si>
+    <t>1K8 1% 0805(2012)</t>
+  </si>
+  <si>
     <t>1K8 0.125W 1% 0805 (2012 Metric)  SMD</t>
   </si>
   <si>
     <t>R1</t>
   </si>
   <si>
+    <t>CMP-1013-00537-1</t>
+  </si>
+  <si>
     <t>ERJ-6ENF1801V</t>
   </si>
   <si>
     <t>P1.80KCCT-ND</t>
+  </si>
+  <si>
+    <t>Trans5_Royer</t>
   </si>
   <si>
     <t>Four-winding Transformer (Non-Ideal)</t>
@@ -245,10 +293,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -564,30 +612,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C5F5B4D-8F07-4456-9C05-22868C05865C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{870E78A6-5FF8-4DDB-B788-64FE0B8821C6}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" customWidth="1"/>
-    <col min="6" max="6" width="24" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" customWidth="1"/>
-    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" customWidth="1"/>
+    <col min="9" max="9" width="24" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" customWidth="1"/>
+    <col min="13" max="13" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -615,247 +664,353 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="4">
+    <row r="2" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="4">
-        <v>2.17</v>
+      <c r="G2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="3">
+        <v>1.74</v>
+      </c>
+      <c r="M2" s="3">
+        <v>1.74</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="M3" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="4">
+      <c r="H4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0.74</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="3">
+        <v>2</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" s="3">
+        <v>1.65</v>
+      </c>
+      <c r="M5" s="3">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="G6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="J6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="4">
-        <v>1.5</v>
+      <c r="K6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="3">
+        <v>2.41</v>
+      </c>
+      <c r="M6" s="3">
+        <v>2.41</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="3" t="s">
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="4">
+      <c r="B7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="4">
-        <v>0.74</v>
-      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="4">
+    <row r="8" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="3">
         <v>2</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="G8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="M8" s="3">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="4">
-        <v>3.3</v>
+      <c r="H9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="M9" s="3">
+        <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="4">
+    <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3">
         <v>1</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="4">
-        <v>2.41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="4">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="4">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" s="4">
-        <v>1.86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I9" s="4">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="4">
-        <v>1</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="58" orientation="landscape" blackAndWhite="1" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="63" orientation="landscape" blackAndWhite="1" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>